<commit_message>
added example notebook on using auto_model_reduction without Data.xlsx
</commit_message>
<xml_diff>
--- a/docs/examples and guides/auto_mlr_notebook/Data.xlsx
+++ b/docs/examples and guides/auto_mlr_notebook/Data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://jlrglobal-my.sharepoint.com/personal/mhidalgo_jaguarlandrover_com/Documents/Projects/ML/docs/examples and guides/auto_mlr_notebook/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mhidalgo\OneDrive\OneDrive - JLR\Projects\CCD\ccd_characterization\ML\docs\examples and guides\auto_mlr_notebook\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{C70CEEA9-DA9F-4A04-86DE-EBCBFB3C4018}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CF80691D-93F4-42B6-942D-FEAF15D24473}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B2A0297-5F1F-4808-A0E6-EC44CA8053EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{C1646789-F2F7-4596-96D5-A1743CEE8B52}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{C1646789-F2F7-4596-96D5-A1743CEE8B52}"/>
   </bookViews>
   <sheets>
     <sheet name="Train Data" sheetId="4" r:id="rId1"/>
@@ -189,21 +189,6 @@
     <t>Run</t>
   </si>
   <si>
-    <t>Roll temperature (°C)</t>
-  </si>
-  <si>
-    <t>Target density (g/cm3)</t>
-  </si>
-  <si>
-    <t>Calculated target porosity (%)</t>
-  </si>
-  <si>
-    <t>C/5-6 (mAh/g)</t>
-  </si>
-  <si>
-    <t>10C (mAh/g)</t>
-  </si>
-  <si>
     <t>A</t>
   </si>
   <si>
@@ -229,6 +214,21 @@
   </si>
   <si>
     <t>Linear</t>
+  </si>
+  <si>
+    <t>roll_temperature</t>
+  </si>
+  <si>
+    <t>density</t>
+  </si>
+  <si>
+    <t>porosity</t>
+  </si>
+  <si>
+    <t>C_5_6</t>
+  </si>
+  <si>
+    <t>_10C</t>
   </si>
 </sst>
 </file>
@@ -689,30 +689,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7017105-9951-4AAA-B498-721790E5798E}">
   <dimension ref="A1:F19"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -1087,29 +1087,29 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:F4"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -1181,10 +1181,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1A90CAD-67BE-406A-8BD7-81EDC587CCAA}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:M6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3:C4"/>
+      <selection activeCell="O9" sqref="O9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1197,7 +1197,7 @@
     <col min="7" max="16384" width="8.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -1205,7 +1205,7 @@
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
@@ -1217,15 +1217,15 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>13</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>18</v>
       </c>
       <c r="D2" s="1">
         <v>85</v>
@@ -1234,18 +1234,18 @@
         <v>145</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>18</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="D3" s="1">
         <v>2.7</v>
@@ -1254,18 +1254,18 @@
         <v>3.2</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>19</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="D4" s="1">
         <v>28</v>
@@ -1274,8 +1274,15 @@
         <v>40</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>14</v>
-      </c>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="I6" s="6"/>
+      <c r="J6" s="6"/>
+      <c r="K6" s="6"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
     </row>
   </sheetData>
   <dataValidations count="2">
@@ -1295,8 +1302,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43A8F6C1-4570-407C-96BE-50A819E04C7D}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B2:B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1316,18 +1323,18 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -1340,18 +1347,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{996A7378-54BB-494D-84D1-CDC0B6ABA572}">
   <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J4" sqref="D4:J33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B1" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>